<commit_message>
Added heuristics check file.
</commit_message>
<xml_diff>
--- a/src/assets/docs/heuristics-evaulation.xlsx
+++ b/src/assets/docs/heuristics-evaulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan.pavic/Documents/Courses/UX &amp; UI/Capstone/coursera-meta-frontend-capstone/src/assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BAF6D4-7F86-F240-A64E-2A8753A9ED0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510DF7CB-7CCA-144B-9B81-B996D14E3362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21240" xr2:uid="{DE46663D-1C1A-484A-8C32-A8A04FF06295}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21240" activeTab="1" xr2:uid="{DE46663D-1C1A-484A-8C32-A8A04FF06295}"/>
   </bookViews>
   <sheets>
     <sheet name="Heuristics  Template 1" sheetId="3" r:id="rId1"/>
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp101.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp102.xml><?xml version="1.0" encoding="utf-8"?>
@@ -813,7 +813,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp119.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,7 +825,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp121.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp122.xml><?xml version="1.0" encoding="utf-8"?>
@@ -833,7 +833,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp123.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp124.xml><?xml version="1.0" encoding="utf-8"?>
@@ -841,7 +841,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp125.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp126.xml><?xml version="1.0" encoding="utf-8"?>
@@ -921,7 +921,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp143.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp144.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,7 +1001,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp161.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp162.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1009,7 +1009,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp163.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp164.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,7 +1017,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp165.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp166.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,7 +1025,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp167.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp168.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1053,7 +1053,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp173.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp174.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1061,7 +1061,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp175.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp176.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1121,7 +1121,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp189.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp191.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp192.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1197,7 +1197,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp205.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp206.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1277,7 +1277,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp223.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp224.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1285,7 +1285,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp225.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp226.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1293,7 +1293,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp227.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp228.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1301,7 +1301,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp229.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1621,7 +1621,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp95.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp96.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1629,7 +1629,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp97.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp98.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,7 +1637,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp99.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17287,8 +17287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0060AC88-6094-42D4-81FE-665911260B88}">
   <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A50" zoomScale="142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17577,20 +17577,32 @@
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
@@ -17623,20 +17635,32 @@
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -17669,20 +17693,32 @@
       <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>39</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17715,6 +17751,9 @@
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
@@ -17723,13 +17762,17 @@
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
-      <c r="E48"/>
+      <c r="E48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="3"/>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
       <c r="K49" s="3"/>
     </row>
     <row r="50" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -17762,15 +17805,24 @@
       <c r="A52" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:11" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
       </c>
       <c r="K54" s="3"/>
     </row>
@@ -17804,20 +17856,32 @@
       <c r="A57" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>52</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -22889,7 +22953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD0F136-7068-4E3B-9BC0-C2290D95C638}">
   <dimension ref="A2:K60"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>

</xml_diff>